<commit_message>
this is my first step to leaarn git
</commit_message>
<xml_diff>
--- a/rft.xlsx
+++ b/rft.xlsx
@@ -19,12 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>refergtrh</t>
   </si>
   <si>
-    <t>tgrt</t>
+    <t>gtyu</t>
+  </si>
+  <si>
+    <t>gf</t>
+  </si>
+  <si>
+    <t>fff</t>
   </si>
 </sst>
 </file>
@@ -342,20 +348,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>